<commit_message>
Update To All Country Files And Master
MaterFile should have all correct calculaions and seperate country files have been corrected also
</commit_message>
<xml_diff>
--- a/Datasets/SeperateCountryFiles/Finland.xlsx
+++ b/Datasets/SeperateCountryFiles/Finland.xlsx
@@ -3551,10 +3551,10 @@
         <v>95</v>
       </c>
       <c r="I63" s="2" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J63" s="2" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="K63" s="2" t="inlineStr">
         <is>

</xml_diff>